<commit_message>
Update for 1-st revision
</commit_message>
<xml_diff>
--- a/Pilot_Results/Pilot_Results.xlsx
+++ b/Pilot_Results/Pilot_Results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
@@ -1181,6 +1181,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="WPS">
   <a:themeElements>
@@ -1439,7 +1446,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="82.0909090909091" customWidth="1"/>
+    <col min="1" max="1" width="72.8181818181818" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="14.4272727272727" customWidth="1"/>
     <col min="4" max="4" width="17.1363636363636" customWidth="1"/>
@@ -2584,7 +2591,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://stackoverflow.com/questions/76144124"/>
+    <hyperlink ref="A3" r:id="rId1" display="https://stackoverflow.com/questions/76144124" tooltip="https://stackoverflow.com/questions/76144124"/>
     <hyperlink ref="A4" r:id="rId2" display="https://stackoverflow.com/questions/76145836"/>
     <hyperlink ref="A5" r:id="rId3" display="https://stackoverflow.com/questions/76146753"/>
     <hyperlink ref="A6" r:id="rId4" display="https://stackoverflow.com/questions/76158645"/>
@@ -2650,6 +2657,7 @@
     <hyperlink ref="A75" r:id="rId64" display="https://github.com/blw-ofag-ufag/eCH-0261/issues/26"/>
     <hyperlink ref="A76" r:id="rId65" display="https://github.com/software-mansion/react-native-screens/issues/1981"/>
     <hyperlink ref="A70" r:id="rId66" display="https://github.com/WordPress/gutenberg/issues/57234"/>
+    <hyperlink ref="A2" r:id="rId67" display="https://stackoverflow.com/questions/77246412"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>